<commit_message>
Update resource utilization diagram with results from the latest bug fix
</commit_message>
<xml_diff>
--- a/documentation/resource_utilization.xlsx
+++ b/documentation/resource_utilization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\Documents\_My_files\Diverse\Programmering\Prosjekter\AES_256_CTR\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0197DA64-1A48-48EC-81D4-02B9D9E7B0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095AE99A-0F04-42C4-8D0C-33B6F31BD5BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D1860934-A991-4C4E-9C78-B5F92E65A6CE}"/>
   </bookViews>
@@ -57,10 +57,10 @@
     <t>dd3a5d3: Before optimizations</t>
   </si>
   <si>
-    <t>cf95cde: Round keys are not shared between Cores.</t>
+    <t>Resource usage with 15 cores</t>
   </si>
   <si>
-    <t>Resource usage with 15 cores</t>
+    <t>4a408d2: Round keys are not shared between Cores.</t>
   </si>
 </sst>
 </file>
@@ -431,25 +431,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>3354</c:v>
+                  <c:v>3356</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4576</c:v>
+                  <c:v>4603</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5800</c:v>
+                  <c:v>5614</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7280</c:v>
+                  <c:v>6986</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8000</c:v>
+                  <c:v>8052</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10801</c:v>
+                  <c:v>10795</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20439</c:v>
+                  <c:v>20514</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -997,10 +997,10 @@
                   <c:v>7660</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9915</c:v>
+                  <c:v>9914</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17338</c:v>
+                  <c:v>17336</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1544,10 +1544,10 @@
                   <c:v>896</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>768</c:v>
+                  <c:v>1280</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>768</c:v>
+                  <c:v>1536</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1280</c:v>
@@ -2100,10 +2100,10 @@
                   <c:v>352</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>352</c:v>
+                  <c:v>608</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>352</c:v>
+                  <c:v>736</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>608</c:v>
@@ -5020,8 +5020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B65E7700-405A-43DB-ADDD-7B45DCEE6BD0}">
   <dimension ref="B1:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5095,7 +5095,7 @@
         <v>1</v>
       </c>
       <c r="J3">
-        <v>3354</v>
+        <v>3356</v>
       </c>
       <c r="K3">
         <v>3437</v>
@@ -5107,19 +5107,19 @@
         <v>352</v>
       </c>
       <c r="O3" s="1">
-        <f>J3/C3-1</f>
-        <v>6.4761904761904798E-2</v>
+        <f t="shared" ref="O3:O6" si="0">(J3/C3-1)*$I3/$H3</f>
+        <v>6.5396825396825342E-2</v>
       </c>
       <c r="P3" s="1">
-        <f>K3/D3-1</f>
+        <f t="shared" ref="P3:P7" si="1">(K3/D3-1)*$I3/$H3</f>
         <v>-3.237612612612617E-2</v>
       </c>
       <c r="Q3" s="1">
-        <f>L3/E3-1</f>
+        <f t="shared" ref="Q3:Q7" si="2">(L3/E3-1)*$I3/$H3</f>
         <v>0</v>
       </c>
       <c r="R3" s="1">
-        <f>M3/F3-1</f>
+        <f t="shared" ref="R3:R7" si="3">(M3/F3-1)*$I3/$H3</f>
         <v>0</v>
       </c>
     </row>
@@ -5147,7 +5147,7 @@
         <v>1.875</v>
       </c>
       <c r="J4">
-        <v>4576</v>
+        <v>4603</v>
       </c>
       <c r="K4">
         <v>4498</v>
@@ -5159,20 +5159,20 @@
         <v>352</v>
       </c>
       <c r="O4" s="1">
-        <f t="shared" ref="O4:O6" si="0">J4/C4-1</f>
-        <v>-5.1999171327946958E-2</v>
+        <f t="shared" si="0"/>
+        <v>-4.3505282784338101E-2</v>
       </c>
       <c r="P4" s="1">
-        <f t="shared" ref="P4:P6" si="1">K4/D4-1</f>
-        <v>-4.9852133502323648E-2</v>
+        <f t="shared" si="1"/>
+        <v>-4.673637515842842E-2</v>
       </c>
       <c r="Q4" s="1">
-        <f t="shared" ref="Q4:Q6" si="2">L4/E4-1</f>
-        <v>-0.125</v>
+        <f t="shared" si="2"/>
+        <v>-0.1171875</v>
       </c>
       <c r="R4" s="1">
-        <f t="shared" ref="R4:R6" si="3">M4/F4-1</f>
-        <v>-0.26666666666666672</v>
+        <f t="shared" si="3"/>
+        <v>-0.25000000000000006</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
@@ -5198,20 +5198,20 @@
         <v>3</v>
       </c>
       <c r="J5">
-        <v>5800</v>
+        <v>5614</v>
       </c>
       <c r="K5">
         <v>5559</v>
       </c>
       <c r="L5">
-        <v>768</v>
+        <v>1280</v>
       </c>
       <c r="M5">
-        <v>352</v>
+        <v>608</v>
       </c>
       <c r="O5" s="1">
         <f t="shared" si="0"/>
-        <v>-0.10824108241082409</v>
+        <v>-0.13683886838868387</v>
       </c>
       <c r="P5" s="1">
         <f t="shared" si="1"/>
@@ -5219,11 +5219,11 @@
       </c>
       <c r="Q5" s="1">
         <f t="shared" si="2"/>
-        <v>-0.4</v>
+        <v>0</v>
       </c>
       <c r="R5" s="1">
         <f t="shared" si="3"/>
-        <v>-0.42105263157894735</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
@@ -5250,32 +5250,32 @@
         <v>3.75</v>
       </c>
       <c r="J6">
-        <v>7280</v>
+        <v>6986</v>
       </c>
       <c r="K6">
         <v>6620</v>
       </c>
       <c r="L6">
-        <v>768</v>
+        <v>1536</v>
       </c>
       <c r="M6">
-        <v>352</v>
+        <v>736</v>
       </c>
       <c r="O6" s="1">
         <f t="shared" si="0"/>
-        <v>-8.8632949424136243E-2</v>
+        <v>-0.11759827240861297</v>
       </c>
       <c r="P6" s="1">
         <f t="shared" si="1"/>
-        <v>-6.7868206139115705E-2</v>
+        <v>-6.3626443255420967E-2</v>
       </c>
       <c r="Q6" s="1">
         <f t="shared" si="2"/>
-        <v>-0.5714285714285714</v>
+        <v>-0.13392857142857148</v>
       </c>
       <c r="R6" s="1">
         <f t="shared" si="3"/>
-        <v>-0.59259259259259256</v>
+        <v>-0.1388888888888889</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
@@ -5301,7 +5301,7 @@
         <v>5</v>
       </c>
       <c r="J7">
-        <v>8000</v>
+        <v>8052</v>
       </c>
       <c r="K7">
         <v>7660</v>
@@ -5313,19 +5313,19 @@
         <v>608</v>
       </c>
       <c r="O7" s="1">
-        <f>J7/C7-1</f>
-        <v>-0.18566775244299671</v>
+        <f>(J7/C7-1)*$I7/$H7</f>
+        <v>-0.18037459283387625</v>
       </c>
       <c r="P7" s="1">
-        <f>K7/D7-1</f>
+        <f t="shared" si="1"/>
         <v>-7.8329924196847589E-2</v>
       </c>
       <c r="Q7" s="1">
-        <f>L7/E7-1</f>
+        <f t="shared" si="2"/>
         <v>-0.2857142857142857</v>
       </c>
       <c r="R7" s="1">
-        <f>M7/F7-1</f>
+        <f t="shared" si="3"/>
         <v>-0.29629629629629628</v>
       </c>
     </row>
@@ -5353,10 +5353,10 @@
         <v>7.5</v>
       </c>
       <c r="J8">
-        <v>10801</v>
+        <v>10795</v>
       </c>
       <c r="K8">
-        <v>9915</v>
+        <v>9914</v>
       </c>
       <c r="L8">
         <v>1280</v>
@@ -5365,20 +5365,20 @@
         <v>608</v>
       </c>
       <c r="O8" s="1">
-        <f>J8/C10-1</f>
-        <v>-0.26678433236032861</v>
+        <f>(J8/C10-1)*$I8/$H8</f>
+        <v>-0.2504921593917589</v>
       </c>
       <c r="P8" s="1">
-        <f>K8/D10-1</f>
-        <v>-0.16456016177957533</v>
+        <f t="shared" ref="P8:R8" si="4">(K8/D10-1)*$I8/$H8</f>
+        <v>-0.15435414560161784</v>
       </c>
       <c r="Q8" s="1">
-        <f>L8/E10-1</f>
-        <v>-0.52416356877323422</v>
+        <f t="shared" si="4"/>
+        <v>-0.49140334572490707</v>
       </c>
       <c r="R8" s="1">
-        <f>M8/F10-1</f>
-        <v>-0.51282051282051277</v>
+        <f t="shared" si="4"/>
+        <v>-0.48076923076923073</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
@@ -5404,10 +5404,10 @@
         <v>15</v>
       </c>
       <c r="J9">
-        <v>20439</v>
+        <v>20514</v>
       </c>
       <c r="K9">
-        <v>17338</v>
+        <v>17336</v>
       </c>
       <c r="L9">
         <v>768</v>
@@ -5416,19 +5416,19 @@
         <v>352</v>
       </c>
       <c r="O9" s="1">
-        <f>J9/C17-1</f>
-        <v>-0.22556077599272506</v>
+        <f>(J9/C17-1)*$I9/$H9</f>
+        <v>-0.22271900575932102</v>
       </c>
       <c r="P9" s="1">
-        <f>K9/D17-1</f>
-        <v>-0.13946793726424456</v>
+        <f t="shared" ref="P9:R9" si="5">(K9/D17-1)*$I9/$H9</f>
+        <v>-0.13956720270001988</v>
       </c>
       <c r="Q9" s="1">
-        <f>L9/E17-1</f>
+        <f t="shared" si="5"/>
         <v>-0.82369146005509641</v>
       </c>
       <c r="R9" s="1">
-        <f>M9/F17-1</f>
+        <f t="shared" si="5"/>
         <v>-0.83589743589743593</v>
       </c>
     </row>
@@ -5570,7 +5570,7 @@
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
@@ -5611,27 +5611,27 @@
         <v>4.1641406486814248E-2</v>
       </c>
       <c r="K22" s="1">
-        <f t="shared" ref="K22" si="4">D22/D$21-1</f>
+        <f t="shared" ref="K22" si="6">D22/D$21-1</f>
         <v>-9.5294818344252574E-2</v>
       </c>
       <c r="L22" s="1">
-        <f t="shared" ref="L22" si="5">E22/E$21-1</f>
+        <f t="shared" ref="L22" si="7">E22/E$21-1</f>
         <v>0</v>
       </c>
       <c r="M22" s="1">
-        <f t="shared" ref="M22" si="6">F22/F$21-1</f>
+        <f t="shared" ref="M22" si="8">F22/F$21-1</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C23">
-        <v>20439</v>
+        <v>20514</v>
       </c>
       <c r="D23">
-        <v>17338</v>
+        <v>17336</v>
       </c>
       <c r="E23">
         <v>768</v>
@@ -5641,18 +5641,18 @@
       </c>
       <c r="J23" s="1">
         <f>C23/C$21-1</f>
-        <v>-0.22556077599272506</v>
+        <v>-0.22271900575932102</v>
       </c>
       <c r="K23" s="1">
-        <f t="shared" ref="K23" si="7">D23/D$21-1</f>
-        <v>-0.13946793726424456</v>
+        <f t="shared" ref="K23" si="9">D23/D$21-1</f>
+        <v>-0.13956720270001988</v>
       </c>
       <c r="L23" s="1">
-        <f t="shared" ref="L23" si="8">E23/E$21-1</f>
+        <f t="shared" ref="L23" si="10">E23/E$21-1</f>
         <v>-0.82369146005509641</v>
       </c>
       <c r="M23" s="1">
-        <f t="shared" ref="M23" si="9">F23/F$21-1</f>
+        <f t="shared" ref="M23" si="11">F23/F$21-1</f>
         <v>-0.83589743589743593</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update resource_utilization.xlsx with new synthesis results
</commit_message>
<xml_diff>
--- a/documentation/resource_utilization.xlsx
+++ b/documentation/resource_utilization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\Documents\_My_files\Diverse\Programmering\Prosjekter\AES_256_CTR\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095AE99A-0F04-42C4-8D0C-33B6F31BD5BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C8592F-35CE-4FBC-B2B9-B13AC2D1D0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D1860934-A991-4C4E-9C78-B5F92E65A6CE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
   <si>
     <t>F7 Muxes</t>
   </si>
@@ -42,42 +42,26 @@
     <t>Number of Cores</t>
   </si>
   <si>
-    <t>Non-sharing of round keys</t>
-  </si>
-  <si>
     <t>Throughput multiplier</t>
   </si>
   <si>
     <t>Old implementation (dd3a5d3)</t>
   </si>
   <si>
-    <t>1f6d486: Eliminate a 128-bit reg</t>
-  </si>
-  <si>
-    <t>dd3a5d3: Before optimizations</t>
-  </si>
-  <si>
     <t>Resource usage with 15 cores</t>
   </si>
   <si>
-    <t>4a408d2: Round keys are not shared between Cores.</t>
+    <t>4a408d2: Non-sharing of round keys</t>
+  </si>
+  <si>
+    <t>954cf5b: Eliminate fifo buffers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0\ %"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,17 +87,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -365,7 +346,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Non-sharing of round keys</c:v>
+                  <c:v>4a408d2: Non-sharing of round keys</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -426,10 +407,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$3:$J$16</c:f>
+              <c:f>Sheet1!$J$3:$J$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>3356</c:v>
                 </c:pt>
@@ -458,6 +439,111 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7379-4E69-915D-26E4F4F40F80}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>954cf5b: Eliminate fifo buffers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$3:$P$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$3:$Q$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3092</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3977</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4866</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6008</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7156</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8800</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15522</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6E5A-4E7D-B61D-F955F3450E9C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -916,7 +1002,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Non-sharing of round keys</c:v>
+                  <c:v>4a408d2: Non-sharing of round keys</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -977,10 +1063,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$3:$K$16</c:f>
+              <c:f>Sheet1!$K$3:$K$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>3437</c:v>
                 </c:pt>
@@ -1009,6 +1095,111 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-839A-4903-BC90-CE37964B40EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>954cf5b: Eliminate fifo buffers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$3:$P$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$3:$R$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2911</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3446</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3981</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4516</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5051</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6244</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4CD7-43AB-913B-86D1DF45704C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1472,7 +1663,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Non-sharing of round keys</c:v>
+                  <c:v>4a408d2: Non-sharing of round keys</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1533,10 +1724,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$3:$L$16</c:f>
+              <c:f>Sheet1!$L$3:$L$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>768</c:v>
                 </c:pt>
@@ -1565,6 +1756,111 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-29CE-4C2C-BB33-25F50E2A2F6B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>954cf5b: Eliminate fifo buffers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$3:$P$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$3:$S$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1536</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1792</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2304</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2560</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DA01-4C25-A522-9784CBF99F37}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2028,7 +2324,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Non-sharing of round keys</c:v>
+                  <c:v>4a408d2: Non-sharing of round keys</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2089,10 +2385,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$M$3:$M$16</c:f>
+              <c:f>Sheet1!$M$3:$M$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>352</c:v>
                 </c:pt>
@@ -2121,6 +2417,111 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-22B5-4224-9591-890C71FB46A4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>954cf5b: Eliminate fifo buffers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$3:$P$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$T$3:$T$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>352</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>608</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>736</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>864</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1120</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1248</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8B6B-4EED-80F4-9E1CF33907D5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4572,14 +4973,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>525780</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4606,16 +5007,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4645,15 +5046,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>502920</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4682,16 +5083,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>396240</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5018,26 +5419,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B65E7700-405A-43DB-ADDD-7B45DCEE6BD0}">
-  <dimension ref="B1:R23"/>
+  <dimension ref="B1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="43.21875" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -5057,7 +5463,7 @@
         <v>4</v>
       </c>
       <c r="I2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J2" t="s">
         <v>2</v>
@@ -5071,8 +5477,26 @@
       <c r="M2" t="s">
         <v>1</v>
       </c>
+      <c r="O2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1</v>
       </c>
@@ -5106,24 +5530,26 @@
       <c r="M3">
         <v>352</v>
       </c>
-      <c r="O3" s="1">
-        <f t="shared" ref="O3:O6" si="0">(J3/C3-1)*$I3/$H3</f>
-        <v>6.5396825396825342E-2</v>
-      </c>
-      <c r="P3" s="1">
-        <f t="shared" ref="P3:P7" si="1">(K3/D3-1)*$I3/$H3</f>
-        <v>-3.237612612612617E-2</v>
-      </c>
-      <c r="Q3" s="1">
-        <f t="shared" ref="Q3:Q7" si="2">(L3/E3-1)*$I3/$H3</f>
-        <v>0</v>
-      </c>
-      <c r="R3" s="1">
-        <f t="shared" ref="R3:R7" si="3">(M3/F3-1)*$I3/$H3</f>
-        <v>0</v>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>3092</v>
+      </c>
+      <c r="R3">
+        <v>2911</v>
+      </c>
+      <c r="S3">
+        <v>768</v>
+      </c>
+      <c r="T3">
+        <v>352</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2</v>
       </c>
@@ -5158,24 +5584,27 @@
       <c r="M4">
         <v>352</v>
       </c>
-      <c r="O4" s="1">
-        <f t="shared" si="0"/>
-        <v>-4.3505282784338101E-2</v>
-      </c>
-      <c r="P4" s="1">
-        <f t="shared" si="1"/>
-        <v>-4.673637515842842E-2</v>
-      </c>
-      <c r="Q4" s="1">
-        <f t="shared" si="2"/>
-        <v>-0.1171875</v>
-      </c>
-      <c r="R4" s="1">
-        <f t="shared" si="3"/>
-        <v>-0.25000000000000006</v>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <f>15/8</f>
+        <v>1.875</v>
+      </c>
+      <c r="Q4">
+        <v>3977</v>
+      </c>
+      <c r="R4">
+        <v>3446</v>
+      </c>
+      <c r="S4">
+        <v>1152</v>
+      </c>
+      <c r="T4">
+        <v>480</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>3</v>
       </c>
@@ -5209,24 +5638,26 @@
       <c r="M5">
         <v>608</v>
       </c>
-      <c r="O5" s="1">
-        <f t="shared" si="0"/>
-        <v>-0.13683886838868387</v>
-      </c>
-      <c r="P5" s="1">
-        <f t="shared" si="1"/>
-        <v>-6.0821084642676104E-2</v>
-      </c>
-      <c r="Q5" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R5" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="O5">
+        <v>3</v>
+      </c>
+      <c r="P5">
+        <v>3</v>
+      </c>
+      <c r="Q5">
+        <v>4866</v>
+      </c>
+      <c r="R5">
+        <v>3981</v>
+      </c>
+      <c r="S5">
+        <v>1280</v>
+      </c>
+      <c r="T5">
+        <v>608</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>4</v>
       </c>
@@ -5261,24 +5692,27 @@
       <c r="M6">
         <v>736</v>
       </c>
-      <c r="O6" s="1">
-        <f t="shared" si="0"/>
-        <v>-0.11759827240861297</v>
-      </c>
-      <c r="P6" s="1">
-        <f t="shared" si="1"/>
-        <v>-6.3626443255420967E-2</v>
-      </c>
-      <c r="Q6" s="1">
-        <f t="shared" si="2"/>
-        <v>-0.13392857142857148</v>
-      </c>
-      <c r="R6" s="1">
-        <f t="shared" si="3"/>
-        <v>-0.1388888888888889</v>
+      <c r="O6">
+        <v>4</v>
+      </c>
+      <c r="P6">
+        <f>15/4</f>
+        <v>3.75</v>
+      </c>
+      <c r="Q6">
+        <v>6008</v>
+      </c>
+      <c r="R6">
+        <v>4516</v>
+      </c>
+      <c r="S6">
+        <v>1536</v>
+      </c>
+      <c r="T6">
+        <v>736</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>5</v>
       </c>
@@ -5312,24 +5746,26 @@
       <c r="M7">
         <v>608</v>
       </c>
-      <c r="O7" s="1">
-        <f>(J7/C7-1)*$I7/$H7</f>
-        <v>-0.18037459283387625</v>
-      </c>
-      <c r="P7" s="1">
-        <f t="shared" si="1"/>
-        <v>-7.8329924196847589E-2</v>
-      </c>
-      <c r="Q7" s="1">
-        <f t="shared" si="2"/>
-        <v>-0.2857142857142857</v>
-      </c>
-      <c r="R7" s="1">
-        <f t="shared" si="3"/>
-        <v>-0.29629629629629628</v>
+      <c r="O7">
+        <v>5</v>
+      </c>
+      <c r="P7">
+        <v>5</v>
+      </c>
+      <c r="Q7">
+        <v>7156</v>
+      </c>
+      <c r="R7">
+        <v>5051</v>
+      </c>
+      <c r="S7">
+        <v>1792</v>
+      </c>
+      <c r="T7">
+        <v>864</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>6</v>
       </c>
@@ -5364,24 +5800,27 @@
       <c r="M8">
         <v>608</v>
       </c>
-      <c r="O8" s="1">
-        <f>(J8/C10-1)*$I8/$H8</f>
-        <v>-0.2504921593917589</v>
-      </c>
-      <c r="P8" s="1">
-        <f t="shared" ref="P8:R8" si="4">(K8/D10-1)*$I8/$H8</f>
-        <v>-0.15435414560161784</v>
-      </c>
-      <c r="Q8" s="1">
-        <f t="shared" si="4"/>
-        <v>-0.49140334572490707</v>
-      </c>
-      <c r="R8" s="1">
-        <f t="shared" si="4"/>
-        <v>-0.48076923076923073</v>
+      <c r="O8">
+        <v>8</v>
+      </c>
+      <c r="P8">
+        <f>15/2</f>
+        <v>7.5</v>
+      </c>
+      <c r="Q8">
+        <v>8800</v>
+      </c>
+      <c r="R8">
+        <v>6244</v>
+      </c>
+      <c r="S8">
+        <v>2304</v>
+      </c>
+      <c r="T8">
+        <v>1120</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>7</v>
       </c>
@@ -5415,24 +5854,26 @@
       <c r="M9">
         <v>352</v>
       </c>
-      <c r="O9" s="1">
-        <f>(J9/C17-1)*$I9/$H9</f>
-        <v>-0.22271900575932102</v>
-      </c>
-      <c r="P9" s="1">
-        <f t="shared" ref="P9:R9" si="5">(K9/D17-1)*$I9/$H9</f>
-        <v>-0.13956720270001988</v>
-      </c>
-      <c r="Q9" s="1">
-        <f t="shared" si="5"/>
-        <v>-0.82369146005509641</v>
-      </c>
-      <c r="R9" s="1">
-        <f t="shared" si="5"/>
-        <v>-0.83589743589743593</v>
+      <c r="O9">
+        <v>15</v>
+      </c>
+      <c r="P9">
+        <v>15</v>
+      </c>
+      <c r="Q9">
+        <v>15522</v>
+      </c>
+      <c r="R9">
+        <v>9768</v>
+      </c>
+      <c r="S9">
+        <v>2560</v>
+      </c>
+      <c r="T9">
+        <v>1248</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>8</v>
       </c>
@@ -5449,7 +5890,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>9</v>
       </c>
@@ -5466,7 +5907,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>10</v>
       </c>
@@ -5483,7 +5924,7 @@
         <v>1504</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>11</v>
       </c>
@@ -5500,7 +5941,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>12</v>
       </c>
@@ -5517,7 +5958,7 @@
         <v>1760</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>13</v>
       </c>
@@ -5534,7 +5975,7 @@
         <v>1888</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>14</v>
       </c>
@@ -5551,7 +5992,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>15</v>
       </c>
@@ -5568,119 +6009,12 @@
         <v>2145</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21">
-        <v>26392</v>
-      </c>
-      <c r="D21">
-        <v>20148</v>
-      </c>
-      <c r="E21">
-        <v>4356</v>
-      </c>
-      <c r="F21">
-        <v>2145</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22">
-        <v>27491</v>
-      </c>
-      <c r="D22">
-        <v>18228</v>
-      </c>
-      <c r="E22">
-        <v>4356</v>
-      </c>
-      <c r="F22">
-        <v>2145</v>
-      </c>
-      <c r="J22" s="1">
-        <f>C22/C$21-1</f>
-        <v>4.1641406486814248E-2</v>
-      </c>
-      <c r="K22" s="1">
-        <f t="shared" ref="K22" si="6">D22/D$21-1</f>
-        <v>-9.5294818344252574E-2</v>
-      </c>
-      <c r="L22" s="1">
-        <f t="shared" ref="L22" si="7">E22/E$21-1</f>
-        <v>0</v>
-      </c>
-      <c r="M22" s="1">
-        <f t="shared" ref="M22" si="8">F22/F$21-1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23">
-        <v>20514</v>
-      </c>
-      <c r="D23">
-        <v>17336</v>
-      </c>
-      <c r="E23">
-        <v>768</v>
-      </c>
-      <c r="F23">
-        <v>352</v>
-      </c>
-      <c r="J23" s="1">
-        <f>C23/C$21-1</f>
-        <v>-0.22271900575932102</v>
-      </c>
-      <c r="K23" s="1">
-        <f t="shared" ref="K23" si="9">D23/D$21-1</f>
-        <v>-0.13956720270001988</v>
-      </c>
-      <c r="L23" s="1">
-        <f t="shared" ref="L23" si="10">E23/E$21-1</f>
-        <v>-0.82369146005509641</v>
-      </c>
-      <c r="M23" s="1">
-        <f t="shared" ref="M23" si="11">F23/F$21-1</f>
-        <v>-0.83589743589743593</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J22:M23">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="num" val="-0.2"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="0.2"/>
-        <color rgb="FF63BE7B"/>
-        <color theme="0"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O3:R9">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="num" val="-0.2"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="0.2"/>
-        <color rgb="FF63BE7B"/>
-        <color theme="0"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>